<commit_message>
Add problem_2 and problem_3 according to problem suite
</commit_message>
<xml_diff>
--- a/problem_file_generator/problem.xlsx
+++ b/problem_file_generator/problem.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinfan/Desktop/INT/INT-Coursework-2021/problem_file_generator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhuoy\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22073A65-87B6-C048-A72D-0B5B740C2400}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B33F272-6B43-4AE7-9E92-528F26DDAEF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39020" yWindow="0" windowWidth="25640" windowHeight="19660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12096" yWindow="1188" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -18,6 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">problem!$A$1:$AC$30</definedName>
+    <definedName name="A">problem!$XDD$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -103,7 +104,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -593,32 +594,32 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="25.8"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" style="5" customWidth="1"/>
-    <col min="2" max="5" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="26.77734375" style="5" customWidth="1"/>
+    <col min="2" max="5" width="10.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
@@ -626,7 +627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -634,7 +635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
@@ -642,12 +643,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="C6" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="5" t="s">
         <v>0</v>
       </c>
@@ -656,7 +657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
@@ -665,7 +666,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -674,7 +675,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
@@ -683,7 +684,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
         <v>2</v>
       </c>
@@ -692,7 +693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
@@ -701,7 +702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
@@ -710,7 +711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
@@ -719,7 +720,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
@@ -728,7 +729,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
@@ -737,7 +738,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2">
       <c r="B19" s="11"/>
     </row>
   </sheetData>
@@ -748,28 +749,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E787929-AF6B-4433-9265-CE7BC92EC712}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="24" max="24" width="4.5" customWidth="1"/>
-    <col min="30" max="30" width="5.5" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="24" max="24" width="4.44140625" customWidth="1"/>
+    <col min="30" max="30" width="5.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="24" customHeight="1">
       <c r="A1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1">
         <v>1</v>
@@ -780,9 +781,27 @@
       <c r="F1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G1">
+        <v>3</v>
+      </c>
+      <c r="H1">
+        <v>3</v>
+      </c>
+      <c r="I1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="24" customHeight="1">
       <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
@@ -791,19 +810,46 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="24" customHeight="1">
       <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="24" customHeight="1">
       <c r="A4">
         <v>1</v>
       </c>
@@ -811,47 +857,315 @@
         <v>1</v>
       </c>
       <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="24" customHeight="1">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="24" customHeight="1">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="24" customHeight="1">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="24" customHeight="1">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="24" customHeight="1">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="24" customHeight="1">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
         <v>2</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="24" customHeight="1">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
         <v>5</v>
       </c>
-      <c r="C5">
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <v>5</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="24" customHeight="1">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="24" customHeight="1">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="24" customHeight="1">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add correct problem files in suite
</commit_message>
<xml_diff>
--- a/problem_file_generator/problem.xlsx
+++ b/problem_file_generator/problem.xlsx
@@ -8,34 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhuoy\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B679DA-3E97-4BA3-B96F-DA48711516DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D1FAE2-FAC9-443B-8B15-942A5560499A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12828" yWindow="2628" windowWidth="17280" windowHeight="8964" tabRatio="619" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
     <sheet name="p69steps" sheetId="3" r:id="rId2"/>
-    <sheet name="p7steps" sheetId="6" r:id="rId3"/>
-    <sheet name="p41steps" sheetId="7" r:id="rId4"/>
+    <sheet name="p41steps" sheetId="7" r:id="rId3"/>
+    <sheet name="p7steps" sheetId="6" r:id="rId4"/>
     <sheet name="p33steps" sheetId="8" r:id="rId5"/>
     <sheet name="p25steps" sheetId="9" r:id="rId6"/>
-    <sheet name="p100steps" sheetId="10" r:id="rId7"/>
+    <sheet name="p117steps" sheetId="10" r:id="rId7"/>
     <sheet name="p119steps" sheetId="11" r:id="rId8"/>
+    <sheet name="p100steps" sheetId="12" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">p100steps!$A$1:$AC$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">p100steps!$A$1:$AC$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">p117steps!$A$1:$AC$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">p119steps!$A$1:$AC$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">p25steps!$A$1:$AC$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">p33steps!$A$1:$AC$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">p41steps!$A$1:$AC$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">p41steps!$A$1:$AC$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">p69steps!$A$1:$AC$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">p7steps!$A$1:$AC$30</definedName>
-    <definedName name="A" localSheetId="6">p100steps!$XDD$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">p7steps!$A$1:$AC$30</definedName>
+    <definedName name="A" localSheetId="8">p100steps!$XDD$9</definedName>
+    <definedName name="A" localSheetId="6">p117steps!$XDD$9</definedName>
     <definedName name="A" localSheetId="7">p119steps!$XDD$9</definedName>
     <definedName name="A" localSheetId="5">p25steps!$XDD$9</definedName>
     <definedName name="A" localSheetId="4">p33steps!$XDD$9</definedName>
-    <definedName name="A" localSheetId="3">p41steps!$XDD$9</definedName>
-    <definedName name="A" localSheetId="2">p7steps!$XDD$9</definedName>
+    <definedName name="A" localSheetId="2">p41steps!$XDD$9</definedName>
+    <definedName name="A" localSheetId="3">p7steps!$XDD$9</definedName>
     <definedName name="A">p69steps!$XDD$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -48,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="29">
   <si>
     <t>Wall</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -291,7 +294,84 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="77">
+  <dxfs count="88">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1267,7 +1347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E787929-AF6B-4433-9265-CE7BC92EC712}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
@@ -1693,39 +1773,39 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="76" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="75" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="1" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="2" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="3" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="4" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="5" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="70" priority="6">
+    <cfRule type="containsBlanks" dxfId="81" priority="6">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="7" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="9" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="10" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1735,470 +1815,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843EA9E7-243A-4D4A-92DC-DF667758F18C}">
-  <dimension ref="A1:I14"/>
-  <sheetViews>
-    <sheetView zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
-    <col min="24" max="24" width="4.44140625" customWidth="1"/>
-    <col min="30" max="30" width="5.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="24" customHeight="1">
-      <c r="A1">
-        <v>3</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>5</v>
-      </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-      <c r="E1">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="24" customHeight="1">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="24" customHeight="1">
-      <c r="A3">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="24" customHeight="1">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="24" customHeight="1">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="24" customHeight="1">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="24" customHeight="1">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="24" customHeight="1">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="24" customHeight="1">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="24" customHeight="1">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="24" customHeight="1">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="24" customHeight="1">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="24" customHeight="1">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="65" priority="11" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="64" priority="1" operator="equal">
-      <formula>9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="2" operator="equal">
-      <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="3" operator="equal">
-      <formula>7</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="4" operator="equal">
-      <formula>6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="5" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="59" priority="6">
-      <formula>LEN(TRIM(A1))=0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="7" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="8" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="9" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="10" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E300F2B5-44F8-43EF-8B9D-57E2DCAC9FBF}">
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -2617,39 +2233,503 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="54" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="53" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="1" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="2" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="3" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="4" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="5" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="48" priority="6">
+    <cfRule type="containsBlanks" dxfId="59" priority="6">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="7" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="9" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="10" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843EA9E7-243A-4D4A-92DC-DF667758F18C}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="24" max="24" width="4.44140625" customWidth="1"/>
+    <col min="30" max="30" width="5.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="24" customHeight="1">
+      <c r="A1">
+        <v>3</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>5</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="24" customHeight="1">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="24" customHeight="1">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="24" customHeight="1">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="24" customHeight="1">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="24" customHeight="1">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="24" customHeight="1">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="24" customHeight="1">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="24" customHeight="1">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="24" customHeight="1">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="24" customHeight="1">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="24" customHeight="1">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="24" customHeight="1">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="24" customHeight="1">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:AD30">
+    <cfRule type="cellIs" dxfId="76" priority="11" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:AD30">
+    <cfRule type="cellIs" dxfId="75" priority="1" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="2" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="3" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="4" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="71" priority="5" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="70" priority="6">
+      <formula>LEN(TRIM(A1))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="7" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="9" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="10" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3088,39 +3168,39 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="43" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="1" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="2" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="3" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="4" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="5" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="37" priority="6">
+    <cfRule type="containsBlanks" dxfId="48" priority="6">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="7" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="9" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="10" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3559,39 +3639,39 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="32" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="2" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="3" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="5" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="26" priority="6">
+    <cfRule type="containsBlanks" dxfId="37" priority="6">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="7" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="9" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="10" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3604,8 +3684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8512A1B1-1679-46C2-A95E-461F4D808028}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1"/>
@@ -3715,7 +3795,7 @@
         <v>17</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="24" customHeight="1">
@@ -3726,7 +3806,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -4048,39 +4128,39 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="15" priority="6">
+    <cfRule type="containsBlanks" dxfId="26" priority="6">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4093,7 +4173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA56F1A-09F4-4338-9C69-419701701940}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
+    <sheetView zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -4519,6 +4599,495 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AD30">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:AD30">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="15" priority="6">
+      <formula>LEN(TRIM(A1))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F14E13-D2F5-48B0-87D4-57165611BEFC}">
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="7" max="7" width="4.109375" customWidth="1"/>
+    <col min="24" max="24" width="4.44140625" customWidth="1"/>
+    <col min="30" max="30" width="5.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="24" customHeight="1">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>3</v>
+      </c>
+      <c r="G1">
+        <v>3</v>
+      </c>
+      <c r="H1">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="24" customHeight="1">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="24" customHeight="1">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="24" customHeight="1">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="24" customHeight="1">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="24" customHeight="1">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="24" customHeight="1">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="24" customHeight="1">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="24" customHeight="1">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="24" customHeight="1">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="24" customHeight="1">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="24" customHeight="1">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="24" customHeight="1">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="24" customHeight="1">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:AD30">
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
add problem file 9
</commit_message>
<xml_diff>
--- a/problem_file_generator/problem.xlsx
+++ b/problem_file_generator/problem.xlsx
@@ -1,44 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10314"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhuoy\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinfan/Desktop/INT/INT-Coursework-2021/problem_file_generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D1FAE2-FAC9-443B-8B15-942A5560499A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AA2E31-E82A-DD46-955D-B4E7A91C97B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12828" yWindow="2628" windowWidth="17280" windowHeight="8964" tabRatio="619" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33080" yWindow="2260" windowWidth="24880" windowHeight="16200" tabRatio="619" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
     <sheet name="p69steps" sheetId="3" r:id="rId2"/>
-    <sheet name="p41steps" sheetId="7" r:id="rId3"/>
-    <sheet name="p7steps" sheetId="6" r:id="rId4"/>
-    <sheet name="p33steps" sheetId="8" r:id="rId5"/>
-    <sheet name="p25steps" sheetId="9" r:id="rId6"/>
-    <sheet name="p117steps" sheetId="10" r:id="rId7"/>
-    <sheet name="p119steps" sheetId="11" r:id="rId8"/>
-    <sheet name="p100steps" sheetId="12" r:id="rId9"/>
+    <sheet name="problem" sheetId="14" r:id="rId3"/>
+    <sheet name="p41steps" sheetId="7" r:id="rId4"/>
+    <sheet name="p7steps" sheetId="6" r:id="rId5"/>
+    <sheet name="p33steps" sheetId="8" r:id="rId6"/>
+    <sheet name="p25steps" sheetId="9" r:id="rId7"/>
+    <sheet name="p117steps" sheetId="10" r:id="rId8"/>
+    <sheet name="p119steps" sheetId="11" r:id="rId9"/>
+    <sheet name="p100steps" sheetId="12" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">p100steps!$A$1:$AC$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">p117steps!$A$1:$AC$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">p119steps!$A$1:$AC$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">p25steps!$A$1:$AC$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">p33steps!$A$1:$AC$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">p41steps!$A$1:$AC$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">p100steps!$A$1:$AC$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">p117steps!$A$1:$AC$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">p119steps!$A$1:$AC$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">p25steps!$A$1:$AC$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">p33steps!$A$1:$AC$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">p41steps!$A$1:$AC$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">p69steps!$A$1:$AC$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">p7steps!$A$1:$AC$30</definedName>
-    <definedName name="A" localSheetId="8">p100steps!$XDD$9</definedName>
-    <definedName name="A" localSheetId="6">p117steps!$XDD$9</definedName>
-    <definedName name="A" localSheetId="7">p119steps!$XDD$9</definedName>
-    <definedName name="A" localSheetId="5">p25steps!$XDD$9</definedName>
-    <definedName name="A" localSheetId="4">p33steps!$XDD$9</definedName>
-    <definedName name="A" localSheetId="2">p41steps!$XDD$9</definedName>
-    <definedName name="A" localSheetId="3">p7steps!$XDD$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">p7steps!$A$1:$AC$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">problem!$A$1:$AC$30</definedName>
+    <definedName name="A" localSheetId="9">p100steps!$XDD$9</definedName>
+    <definedName name="A" localSheetId="7">p117steps!$XDD$9</definedName>
+    <definedName name="A" localSheetId="8">p119steps!$XDD$9</definedName>
+    <definedName name="A" localSheetId="6">p25steps!$XDD$9</definedName>
+    <definedName name="A" localSheetId="5">p33steps!$XDD$9</definedName>
+    <definedName name="A" localSheetId="3">p41steps!$XDD$9</definedName>
+    <definedName name="A" localSheetId="4">p7steps!$XDD$9</definedName>
+    <definedName name="A" localSheetId="2">problem!$XDD$9</definedName>
     <definedName name="A">p69steps!$XDD$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -51,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="29">
   <si>
     <t>Wall</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -161,7 +164,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,7 +297,84 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="88">
+  <dxfs count="99">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1190,16 +1270,16 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="25.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" style="5" customWidth="1"/>
-    <col min="2" max="5" width="10.77734375" style="5"/>
+    <col min="1" max="1" width="26.83203125" style="5" customWidth="1"/>
+    <col min="2" max="5" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -1207,23 +1287,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -1231,7 +1311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
@@ -1239,12 +1319,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>0</v>
       </c>
@@ -1253,7 +1333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
@@ -1262,7 +1342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -1271,7 +1351,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
@@ -1280,7 +1360,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>2</v>
       </c>
@@ -1289,7 +1369,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
@@ -1298,7 +1378,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
@@ -1307,7 +1387,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
@@ -1316,7 +1396,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
@@ -1325,7 +1405,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
@@ -1334,12 +1414,501 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F14E13-D2F5-48B0-87D4-57165611BEFC}">
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="7" max="7" width="4.1640625" customWidth="1"/>
+    <col min="24" max="24" width="4.5" customWidth="1"/>
+    <col min="30" max="30" width="5.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>3</v>
+      </c>
+      <c r="G1">
+        <v>3</v>
+      </c>
+      <c r="H1">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:AD30">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:AD30">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="4" priority="6">
+      <formula>LEN(TRIM(A1))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1347,18 +1916,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E787929-AF6B-4433-9265-CE7BC92EC712}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView topLeftCell="A3" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
-    <col min="24" max="24" width="4.44140625" customWidth="1"/>
-    <col min="30" max="30" width="5.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="24" max="24" width="4.5" customWidth="1"/>
+    <col min="30" max="30" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" customHeight="1">
+    <row r="1" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>3</v>
       </c>
@@ -1387,7 +1956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="24" customHeight="1">
+    <row r="2" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1416,7 +1985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="24" customHeight="1">
+    <row r="3" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1448,7 +2017,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="24" customHeight="1">
+    <row r="4" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1480,7 +2049,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="24" customHeight="1">
+    <row r="5" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1509,7 +2078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="24" customHeight="1">
+    <row r="6" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1538,7 +2107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="24" customHeight="1">
+    <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1567,7 +2136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="24" customHeight="1">
+    <row r="8" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1596,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="24" customHeight="1">
+    <row r="9" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1625,7 +2194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="24" customHeight="1">
+    <row r="10" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1654,7 +2223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="24" customHeight="1">
+    <row r="11" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1683,7 +2252,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="24" customHeight="1">
+    <row r="12" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1712,7 +2281,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="24" customHeight="1">
+    <row r="13" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1741,7 +2310,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="24" customHeight="1">
+    <row r="14" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1815,6 +2384,409 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C6CB5C-BFBC-9942-A609-8D05D66518E6}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="6" max="6" width="4.83203125" customWidth="1"/>
+    <col min="7" max="7" width="5.5" customWidth="1"/>
+    <col min="24" max="24" width="4.5" customWidth="1"/>
+    <col min="30" max="30" width="5.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="F1">
+        <v>1</v>
+      </c>
+      <c r="G1">
+        <v>1</v>
+      </c>
+      <c r="H1">
+        <v>1</v>
+      </c>
+      <c r="I1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:AD30">
+    <cfRule type="cellIs" dxfId="98" priority="11" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:AD30">
+    <cfRule type="cellIs" dxfId="97" priority="1" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="2" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="3" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="4" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="5" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="92" priority="6">
+      <formula>LEN(TRIM(A1))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="91" priority="7" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="9" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="10" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E300F2B5-44F8-43EF-8B9D-57E2DCAC9FBF}">
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -1822,16 +2794,16 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
-    <col min="6" max="6" width="4.88671875" customWidth="1"/>
-    <col min="7" max="7" width="5.5546875" customWidth="1"/>
-    <col min="24" max="24" width="4.44140625" customWidth="1"/>
-    <col min="30" max="30" width="5.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="6" max="6" width="4.83203125" customWidth="1"/>
+    <col min="7" max="7" width="5.5" customWidth="1"/>
+    <col min="24" max="24" width="4.5" customWidth="1"/>
+    <col min="30" max="30" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24" customHeight="1">
+    <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1857,7 +2829,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="24" customHeight="1">
+    <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1886,7 +2858,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="24" customHeight="1">
+    <row r="3" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1915,7 +2887,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="24" customHeight="1">
+    <row r="4" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1941,7 +2913,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="24" customHeight="1">
+    <row r="5" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1970,7 +2942,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="24" customHeight="1">
+    <row r="6" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1999,7 +2971,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="24" customHeight="1">
+    <row r="7" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -2028,7 +3000,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="24" customHeight="1">
+    <row r="8" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -2057,7 +3029,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="24" customHeight="1">
+    <row r="9" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2086,7 +3058,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="24" customHeight="1">
+    <row r="10" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2115,7 +3087,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="24" customHeight="1">
+    <row r="11" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -2144,7 +3116,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="24" customHeight="1">
+    <row r="12" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -2173,7 +3145,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="24" customHeight="1">
+    <row r="13" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -2202,7 +3174,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="24" customHeight="1">
+    <row r="14" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2233,39 +3205,39 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="65" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="64" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="1" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="2" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="3" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="4" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="5" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="59" priority="6">
+    <cfRule type="containsBlanks" dxfId="70" priority="6">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="7" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="9" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="10" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2274,7 +3246,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843EA9E7-243A-4D4A-92DC-DF667758F18C}">
   <dimension ref="A1:I14"/>
   <sheetViews>
@@ -2282,14 +3254,14 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
-    <col min="24" max="24" width="4.44140625" customWidth="1"/>
-    <col min="30" max="30" width="5.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="24" max="24" width="4.5" customWidth="1"/>
+    <col min="30" max="30" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" customHeight="1">
+    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>3</v>
       </c>
@@ -2318,7 +3290,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="24" customHeight="1">
+    <row r="2" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2347,7 +3319,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="24" customHeight="1">
+    <row r="3" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>5</v>
       </c>
@@ -2376,7 +3348,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2405,7 +3377,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="24" customHeight="1">
+    <row r="5" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2434,7 +3406,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="24" customHeight="1">
+    <row r="6" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2463,7 +3435,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="24" customHeight="1">
+    <row r="7" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -2492,7 +3464,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="24" customHeight="1">
+    <row r="8" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -2521,7 +3493,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="24" customHeight="1">
+    <row r="9" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2550,7 +3522,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="24" customHeight="1">
+    <row r="10" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2579,7 +3551,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="24" customHeight="1">
+    <row r="11" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -2608,7 +3580,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="24" customHeight="1">
+    <row r="12" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -2637,7 +3609,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="24" customHeight="1">
+    <row r="13" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -2666,7 +3638,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="24" customHeight="1">
+    <row r="14" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2697,39 +3669,39 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="76" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="75" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="1" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="2" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="3" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="4" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="5" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="70" priority="6">
+    <cfRule type="containsBlanks" dxfId="59" priority="6">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="7" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="9" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="10" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2738,7 +3710,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB86B738-3550-4DD4-8233-98BC8BEAA9D7}">
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -2746,15 +3718,15 @@
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
     <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="4.44140625" customWidth="1"/>
-    <col min="30" max="30" width="5.44140625" customWidth="1"/>
+    <col min="24" max="24" width="4.5" customWidth="1"/>
+    <col min="30" max="30" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24" customHeight="1">
+    <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>0</v>
       </c>
@@ -2783,7 +3755,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="24" customHeight="1">
+    <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2815,7 +3787,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="24" customHeight="1">
+    <row r="3" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>6</v>
       </c>
@@ -2847,7 +3819,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="24" customHeight="1">
+    <row r="4" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2876,7 +3848,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="24" customHeight="1">
+    <row r="5" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0</v>
       </c>
@@ -2905,7 +3877,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="24" customHeight="1">
+    <row r="6" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2934,7 +3906,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="24" customHeight="1">
+    <row r="7" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -2963,7 +3935,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="24" customHeight="1">
+    <row r="8" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -2992,7 +3964,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="24" customHeight="1">
+    <row r="9" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -3021,7 +3993,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="24" customHeight="1">
+    <row r="10" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -3050,7 +4022,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="24" customHeight="1">
+    <row r="11" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -3079,7 +4051,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="24" customHeight="1">
+    <row r="12" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3108,7 +4080,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="24" customHeight="1">
+    <row r="13" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -3137,7 +4109,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="24" customHeight="1">
+    <row r="14" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -3209,7 +4181,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8DD75B-A8D3-4628-B0E1-EFFFD147E32F}">
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -3217,15 +4189,15 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
     <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="4.44140625" customWidth="1"/>
-    <col min="30" max="30" width="5.44140625" customWidth="1"/>
+    <col min="24" max="24" width="4.5" customWidth="1"/>
+    <col min="30" max="30" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24" customHeight="1">
+    <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -3254,7 +4226,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="24" customHeight="1">
+    <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3286,7 +4258,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="24" customHeight="1">
+    <row r="3" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3318,7 +4290,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="24" customHeight="1">
+    <row r="4" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
@@ -3347,7 +4319,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="24" customHeight="1">
+    <row r="5" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0</v>
       </c>
@@ -3376,7 +4348,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="24" customHeight="1">
+    <row r="6" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -3405,7 +4377,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="24" customHeight="1">
+    <row r="7" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3434,7 +4406,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="24" customHeight="1">
+    <row r="8" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -3463,7 +4435,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="24" customHeight="1">
+    <row r="9" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -3492,7 +4464,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="24" customHeight="1">
+    <row r="10" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -3521,7 +4493,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="24" customHeight="1">
+    <row r="11" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -3550,7 +4522,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="24" customHeight="1">
+    <row r="12" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3579,7 +4551,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="24" customHeight="1">
+    <row r="13" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -3608,7 +4580,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="24" customHeight="1">
+    <row r="14" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -3672,495 +4644,6 @@
       <formula>3</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="33" priority="10" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8512A1B1-1679-46C2-A95E-461F4D808028}">
-  <dimension ref="A1:L14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
-    <col min="7" max="7" width="4.109375" customWidth="1"/>
-    <col min="24" max="24" width="4.44140625" customWidth="1"/>
-    <col min="30" max="30" width="5.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="24" customHeight="1">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-      <c r="E1">
-        <v>1</v>
-      </c>
-      <c r="F1">
-        <v>1</v>
-      </c>
-      <c r="G1">
-        <v>1</v>
-      </c>
-      <c r="H1">
-        <v>1</v>
-      </c>
-      <c r="I1">
-        <v>1</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="24" customHeight="1">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>5</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="24" customHeight="1">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>5</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="24" customHeight="1">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>5</v>
-      </c>
-      <c r="I4">
-        <v>5</v>
-      </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="24" customHeight="1">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="24" customHeight="1">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6">
-        <v>3</v>
-      </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="24" customHeight="1">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="24" customHeight="1">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="24" customHeight="1">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="24" customHeight="1">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="24" customHeight="1">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="24" customHeight="1">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="24" customHeight="1">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="24" customHeight="1">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="32" priority="11" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
-      <formula>9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
-      <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
-      <formula>7</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
-      <formula>6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="26" priority="6">
-      <formula>LEN(TRIM(A1))=0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="8" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4170,6 +4653,495 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8512A1B1-1679-46C2-A95E-461F4D808028}">
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="7" max="7" width="4.1640625" customWidth="1"/>
+    <col min="24" max="24" width="4.5" customWidth="1"/>
+    <col min="30" max="30" width="5.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="F1">
+        <v>1</v>
+      </c>
+      <c r="G1">
+        <v>1</v>
+      </c>
+      <c r="H1">
+        <v>1</v>
+      </c>
+      <c r="I1">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:AD30">
+    <cfRule type="cellIs" dxfId="32" priority="11" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:AD30">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="26" priority="6">
+      <formula>LEN(TRIM(A1))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA56F1A-09F4-4338-9C69-419701701940}">
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -4177,15 +5149,15 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
-    <col min="7" max="7" width="4.44140625" customWidth="1"/>
-    <col min="24" max="24" width="4.44140625" customWidth="1"/>
-    <col min="30" max="30" width="5.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="7" max="7" width="4.5" customWidth="1"/>
+    <col min="24" max="24" width="4.5" customWidth="1"/>
+    <col min="30" max="30" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="24" customHeight="1">
+    <row r="1" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>0</v>
       </c>
@@ -4214,7 +5186,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="24" customHeight="1">
+    <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4246,7 +5218,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="24" customHeight="1">
+    <row r="3" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4278,7 +5250,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="24" customHeight="1">
+    <row r="4" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
@@ -4307,7 +5279,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="24" customHeight="1">
+    <row r="5" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4336,7 +5308,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="24" customHeight="1">
+    <row r="6" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0</v>
       </c>
@@ -4365,7 +5337,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="24" customHeight="1">
+    <row r="7" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -4394,7 +5366,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="24" customHeight="1">
+    <row r="8" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -4423,7 +5395,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="24" customHeight="1">
+    <row r="9" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -4452,7 +5424,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="24" customHeight="1">
+    <row r="10" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -4481,7 +5453,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="24" customHeight="1">
+    <row r="11" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -4510,7 +5482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="24" customHeight="1">
+    <row r="12" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -4539,7 +5511,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="24" customHeight="1">
+    <row r="13" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -4568,7 +5540,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="24" customHeight="1">
+    <row r="14" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -4632,495 +5604,6 @@
       <formula>3</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F14E13-D2F5-48B0-87D4-57165611BEFC}">
-  <dimension ref="A1:L14"/>
-  <sheetViews>
-    <sheetView zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="24" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
-    <col min="7" max="7" width="4.109375" customWidth="1"/>
-    <col min="24" max="24" width="4.44140625" customWidth="1"/>
-    <col min="30" max="30" width="5.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="24" customHeight="1">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-      <c r="E1">
-        <v>3</v>
-      </c>
-      <c r="F1">
-        <v>3</v>
-      </c>
-      <c r="G1">
-        <v>3</v>
-      </c>
-      <c r="H1">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="24" customHeight="1">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="24" customHeight="1">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="24" customHeight="1">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="24" customHeight="1">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="24" customHeight="1">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="24" customHeight="1">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="24" customHeight="1">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="24" customHeight="1">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="24" customHeight="1">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="24" customHeight="1">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="24" customHeight="1">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="24" customHeight="1">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="24" customHeight="1">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AD30">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
-      <formula>9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
-      <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
-      <formula>7</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
-      <formula>6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="4" priority="6">
-      <formula>LEN(TRIM(A1))=0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>